<commit_message>
feat: connect view feature to main function
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="회원 정보" r:id="rId3" sheetId="1"/>
+    <sheet name="자기소개서" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>사진</t>
   </si>
@@ -30,6 +31,57 @@
   </si>
   <si>
     <t>생년월일</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>졸엽년도</t>
+  </si>
+  <si>
+    <t>학교명</t>
+  </si>
+  <si>
+    <t>전공</t>
+  </si>
+  <si>
+    <t>졸업여부</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>근무기간</t>
+  </si>
+  <si>
+    <t>근무처</t>
+  </si>
+  <si>
+    <t>담당업무</t>
+  </si>
+  <si>
+    <t>근속연수</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -72,9 +124,52 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -100,7 +195,121 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: working on README.md
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>사진</t>
   </si>
@@ -66,6 +66,9 @@
     <t>e</t>
   </si>
   <si>
+    <t>r</t>
+  </si>
+  <si>
     <t>근무기간</t>
   </si>
   <si>
@@ -78,10 +81,12 @@
     <t>근속연수</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qwewqrqwrwq
+sdafasdfasdf
+</t>
   </si>
 </sst>
 </file>
@@ -134,10 +139,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -155,7 +160,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="800100"/>
+          <a:ext cx="533400" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -174,6 +179,9 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="12.375" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -195,7 +203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="95.0" customHeight="true">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -259,24 +267,24 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -309,7 +317,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: photograph file name input feature
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>사진</t>
   </si>
@@ -63,29 +63,22 @@
     <t>w</t>
   </si>
   <si>
-    <t>e</t>
+    <t>근무기간</t>
+  </si>
+  <si>
+    <t>근무처</t>
+  </si>
+  <si>
+    <t>담당업무</t>
+  </si>
+  <si>
+    <t>근속연수</t>
   </si>
   <si>
     <t>r</t>
   </si>
   <si>
-    <t>근무기간</t>
-  </si>
-  <si>
-    <t>근무처</t>
-  </si>
-  <si>
-    <t>담당업무</t>
-  </si>
-  <si>
-    <t>근속연수</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qwewqrqwrwq
-sdafasdfasdf
+    <t xml:space="preserve">asdfasdf
 </t>
   </si>
 </sst>
@@ -123,8 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -174,7 +170,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -253,55 +249,27 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -319,8 +287,8 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>23</v>
+      <c r="A1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: self introduction column size
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>사진</t>
   </si>
@@ -63,6 +63,9 @@
     <t>w</t>
   </si>
   <si>
+    <t>e</t>
+  </si>
+  <si>
     <t>근무기간</t>
   </si>
   <si>
@@ -78,7 +81,12 @@
     <t>r</t>
   </si>
   <si>
-    <t xml:space="preserve">asdfasdf
+    <t>t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdfdsafdasfads
+dsafdsafsadfdsaf
+asdgsdavsvasvasdv
 </t>
   </si>
 </sst>
@@ -170,7 +178,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -249,27 +257,55 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -285,10 +321,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="17.609375" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
+      <c r="A1" t="s" s="1">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: refactor image insert method in controller
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>사진</t>
   </si>
@@ -81,12 +81,9 @@
     <t>r</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asdfdsafdasfads
-dsafdsafsadfdsaf
-asdgsdavsvasvasdv
+    <t xml:space="preserve">asdjfkldsajfkl
+adskfldskjajfkds
+asdjkfldsjkfjlasdkjflkasdjf
 </t>
   </si>
 </sst>
@@ -164,7 +161,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="533400" cy="190500"/>
+          <a:ext cx="819150" cy="1209675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -178,7 +175,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -207,7 +204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="95.0" customHeight="true">
+    <row r="2" ht="95.25" customHeight="true">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -292,20 +289,6 @@
       </c>
       <c r="D7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -322,12 +305,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="17.609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="22.515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add resize column feature on resume sheet(0)
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>사진</t>
   </si>
@@ -33,19 +33,19 @@
     <t>생년월일</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>김원상</t>
+  </si>
+  <si>
+    <t>kimwonsang@gmail.com</t>
+  </si>
+  <si>
+    <t>서울특별시 관막구</t>
+  </si>
+  <si>
+    <t>010-1111-2345</t>
+  </si>
+  <si>
+    <t>1991-01-01</t>
   </si>
   <si>
     <t>졸엽년도</t>
@@ -60,10 +60,25 @@
     <t>졸업여부</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>e</t>
+    <t>2018년</t>
+  </si>
+  <si>
+    <t>행복대학교</t>
+  </si>
+  <si>
+    <t>융합생명정보</t>
+  </si>
+  <si>
+    <t>졸업</t>
+  </si>
+  <si>
+    <t>2010년</t>
+  </si>
+  <si>
+    <t>해울대고등학교</t>
+  </si>
+  <si>
+    <t>자연과학</t>
   </si>
   <si>
     <t>근무기간</t>
@@ -78,12 +93,34 @@
     <t>근속연수</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asdjfkldsajfkl
-adskfldskjajfkds
-asdjkfldsjkfjlasdkjflkasdjf
+    <t>멜엔피솔루션</t>
+  </si>
+  <si>
+    <t>경기도일산</t>
+  </si>
+  <si>
+    <t>개발팀장</t>
+  </si>
+  <si>
+    <t>6개월</t>
+  </si>
+  <si>
+    <t>인셀레브</t>
+  </si>
+  <si>
+    <t>강남구</t>
+  </si>
+  <si>
+    <t>선임연구원</t>
+  </si>
+  <si>
+    <t>3년6개월</t>
+  </si>
+  <si>
+    <t xml:space="preserve">안녕하세요 저는 ~~~~ 입니다.
+앞으로 더 나은 개발자가 되기 위해 ~~~한 점을 계획하고 있습니다.
+제가 이전에 수행했던 프로젝트는 ~~~한 점에서 어려운 면이 있었으나 ~~~한 과정으로 극복하였습니다.
+감사합니다.
 </t>
   </si>
 </sst>
@@ -175,13 +212,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="12.375" customWidth="true"/>
+    <col min="1" max="1" width="11.046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.734375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="22.66015625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.83203125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.390625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.33984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -240,55 +282,69 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -305,12 +361,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="22.515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="77.83984375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: add try-with-resources on controller
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>사진</t>
   </si>
@@ -33,19 +33,19 @@
     <t>생년월일</t>
   </si>
   <si>
-    <t>김원상</t>
-  </si>
-  <si>
-    <t>kimwonsang@gmail.com</t>
-  </si>
-  <si>
-    <t>서울특별시 관악규</t>
-  </si>
-  <si>
-    <t>010-1111-2222</t>
-  </si>
-  <si>
-    <t>1991-02-02</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>졸엽년도</t>
@@ -60,25 +60,10 @@
     <t>졸업여부</t>
   </si>
   <si>
-    <t>2018년</t>
-  </si>
-  <si>
-    <t>경북대학교</t>
-  </si>
-  <si>
-    <t>윤합생명정보</t>
-  </si>
-  <si>
-    <t>졸업</t>
-  </si>
-  <si>
-    <t>2010년</t>
-  </si>
-  <si>
-    <t>해울대고등학교</t>
-  </si>
-  <si>
-    <t>자연과학</t>
+    <t>w</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
   <si>
     <t>근무기간</t>
@@ -93,25 +78,14 @@
     <t>근속연수</t>
   </si>
   <si>
-    <t>6개월</t>
-  </si>
-  <si>
-    <t>경기도일산</t>
-  </si>
-  <si>
-    <t>개발팀장</t>
-  </si>
-  <si>
-    <t>3년6개월</t>
-  </si>
-  <si>
-    <t>강남구</t>
-  </si>
-  <si>
-    <t>선임연구원</t>
-  </si>
-  <si>
-    <t xml:space="preserve">안녕하십니까 김원상입니다.
+    <t>r</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ㄴㅇㄻㄴㅇㄻㄴㄹㅇ
+ㅁㄴㅇㄹㅇㄴㅁㄹㅇㅁㄴㄹ
 </t>
   </si>
 </sst>
@@ -209,12 +183,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="8.0234375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.734375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="22.66015625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.83203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.390625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.33984375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="7.671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="5.98828125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="7.671875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="7.671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="7.671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -273,69 +247,69 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -352,12 +326,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="22.0859375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="21.16796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: delete IOException on main function
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>사진</t>
   </si>
@@ -81,11 +81,9 @@
     <t>r</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ㄴㅇㄻㄴㅇㄻㄴㄹㅇ
-ㅁㄴㅇㄹㅇㄴㅁㄹㅇㅁㄴㄹ
+    <t xml:space="preserve">asdfdsafasdfjlk
+asdjfjklsdajckldas
+dsanvkfdsaklcasdk
 </t>
   </si>
 </sst>
@@ -177,7 +175,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -286,7 +284,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -296,20 +294,6 @@
       </c>
       <c r="D7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -326,12 +310,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="21.16796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="17.16796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>